<commit_message>
Generated javadoc Moved GuiController to GUI class Made more tests for Math class
</commit_message>
<xml_diff>
--- a/metrics_to_compare/ES-2Sem-2021-Grupo24_compare_metrics.xlsx
+++ b/metrics_to_compare/ES-2Sem-2021-Grupo24_compare_metrics.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="139">
   <si>
     <t>MethodID</t>
   </si>
@@ -47,313 +47,370 @@
     <t>is_Long_Method</t>
   </si>
   <si>
+    <t>codeSmells</t>
+  </si>
+  <si>
+    <t>CodeSmellsComparator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getOriginalLines()</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getToCompareLines()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> String, String, String&gt;&gt; getValuesToCompare()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> main(String[])</t>
+  </si>
+  <si>
+    <t>CodeSmellsCreator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> createCodeSmellsXlsxFile(File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> addCodeSmellsToXlsx(File)</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> createHeaderCodeSmellsXlsx(XSSFRow)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> addRowCodeSmellsXlsx(XSSFRow, MethodMetrics)</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getRegras()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> initialize()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> openProject()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setExelOriginal(File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setExcelToCompare(File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chooseExcelToCompare()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chooseExcelOriginal()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> compareExcels()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> isProjectSelected()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> createCodeSmell()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> addRuleToHistory()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> removeRuleFromHistory()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> changeRuleFromHistory()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> finishChangeRuleFromHistory()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getRule()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clearGUIElements()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> updateGUIElements(String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> updateGUIElements(File)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writeCharacteristicsGUI(ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writeCodeSmellsGUI(ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> showInformationMessage(String, String, Alert.AlertType)</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> start(Stage)</t>
+  </si>
+  <si>
     <t>metrics</t>
   </si>
   <si>
+    <t>MethodMetrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getClassOfMethod()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getId()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getPackageOfMethod()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMethod()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setMetric(Metric, int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMetric(Metric)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> verifyRuleset(List&lt;Rule&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getNom_class()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setNom_class(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getLoc_class()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setLoc_class(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getWmc_class()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setWmc_class(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getLoc_method()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setLoc_method(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getCyclo_method()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setCyclo_method(int)</t>
+  </si>
+  <si>
     <t>MetricExtractor</t>
   </si>
   <si>
-    <t>public Path getSrcpath()</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>public void setSrcpath(Path srcpath)</t>
-  </si>
-  <si>
-    <t>public List&lt;MethodMetrics&gt; ExtractMetrics() throws IOException</t>
-  </si>
-  <si>
-    <t>public void joinMetrics(List&lt;MethodMetrics&gt; methodMetrics, List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; metrics, Metric metricEnum)</t>
-  </si>
-  <si>
-    <t>public static List&lt;CompilationUnit&gt; CreateCompilationUnits(Path dirPath) throws IOException</t>
-  </si>
-  <si>
-    <t>public List&lt;CompilationUnit&gt; CreateCompilationUnits() throws IOException</t>
-  </si>
-  <si>
-    <t>private static PackageDeclaration ConvertOptionalToActual(Optional&lt;PackageDeclaration&gt; packageD)</t>
-  </si>
-  <si>
-    <t>private static void PrintQuad(Iterable&lt;? extends Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; quadruples)</t>
-  </si>
-  <si>
-    <t>public List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; NOM_class(List&lt;CompilationUnit&gt; compilationUnits)</t>
-  </si>
-  <si>
-    <t>public List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; CYCLO_method(List&lt;CompilationUnit&gt; compilationUnits)</t>
-  </si>
-  <si>
-    <t>public List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; WMC_class(List&lt;CompilationUnit&gt; compilationUnits)</t>
-  </si>
-  <si>
-    <t>public List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; LOC_method(List&lt;CompilationUnit&gt; compilationUnits)</t>
-  </si>
-  <si>
-    <t>public List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; LOC_class(List&lt;CompilationUnit&gt; compilationUnits)</t>
-  </si>
-  <si>
-    <t>private int countLines(String s)</t>
-  </si>
-  <si>
-    <t>MethodMetrics</t>
-  </si>
-  <si>
-    <t>public ClassOrInterfaceDeclaration getClassOfMethod()</t>
-  </si>
-  <si>
-    <t>public int getId()</t>
-  </si>
-  <si>
-    <t>public PackageDeclaration getPackageOfMethod()</t>
-  </si>
-  <si>
-    <t>public MethodDeclaration getMethod()</t>
-  </si>
-  <si>
-    <t>public void setMetric(Metric metric, int value) throws NoSuchElementException</t>
-  </si>
-  <si>
-    <t>public int getMetric(Metric metric) throws NoSuchElementException</t>
-  </si>
-  <si>
-    <t>public String verifyRuleset(List&lt;Rule&gt; rules)</t>
-  </si>
-  <si>
-    <t>private int getNom_class()</t>
-  </si>
-  <si>
-    <t>private void setNom_class(int nom_class)</t>
-  </si>
-  <si>
-    <t>private int getLoc_class()</t>
-  </si>
-  <si>
-    <t>private void setLoc_class(int loc_class)</t>
-  </si>
-  <si>
-    <t>private int getWmc_class()</t>
-  </si>
-  <si>
-    <t>private void setWmc_class(int wmc_class)</t>
-  </si>
-  <si>
-    <t>private int getLoc_method()</t>
-  </si>
-  <si>
-    <t>private void setLoc_method(int loc_method)</t>
-  </si>
-  <si>
-    <t>private int getCyclo_method()</t>
-  </si>
-  <si>
-    <t>private void setCyclo_method(int cyclo_method)</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>public void start(Stage primaryStage) throws Exception</t>
-  </si>
-  <si>
-    <t>public static void main(String[] args)</t>
+    <t xml:space="preserve"> getSrcpath()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setSrcpath(Path)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ExtractMetrics()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> joinMetrics(List&lt;MethodMetrics&gt;, List&lt;Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt;, Metric)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CreateCompilationUnits(Path)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CreateCompilationUnits()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ConvertOptionalToActual(Optional&lt;PackageDeclaration&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PrettyPrintQuad(Iterable&lt;? extends Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PrettyPrintQuad(Quadruple&lt;PackageDeclaration, ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; NOM_class(List&lt;CompilationUnit&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; CYCLO_method(List&lt;CompilationUnit&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getComplexity(MethodDeclaration, int, Class&lt;T&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; WMC_class(List&lt;CompilationUnit&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; LOC_method(List&lt;CompilationUnit&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ClassOrInterfaceDeclaration, MethodDeclaration, Integer&gt;&gt; LOC_class(List&lt;CompilationUnit&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> countLines(String)</t>
   </si>
   <si>
     <t>readers</t>
   </si>
   <si>
+    <t>ExelReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> read(File)</t>
+  </si>
+  <si>
     <t>JavaReader</t>
   </si>
   <si>
-    <t>public void read()</t>
-  </si>
-  <si>
-    <t>ExelReader</t>
-  </si>
-  <si>
-    <t>public ArrayList&lt;String&gt; read()</t>
-  </si>
-  <si>
-    <t>CodeSmells</t>
-  </si>
-  <si>
-    <t>public void createCodeSmellsXlsxFile(File dir) throws IOException</t>
-  </si>
-  <si>
-    <t>public void addCodeSmellsToXlsx(File dir) throws IOException</t>
-  </si>
-  <si>
-    <t>private void createHeaderCodeSmellsXlsx(XSSFRow rowhead)</t>
-  </si>
-  <si>
-    <t>private void addRowCodeSmellsXlsx(XSSFRow row, MethodMetrics method)</t>
+    <t xml:space="preserve"> read()</t>
+  </si>
+  <si>
+    <t>rules</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getRule1()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getRule2()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getOperation()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getSmell()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMetric(SubRule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMetricOperation(SubRule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMetricValue(SubRule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> passesRule(MethodMetrics)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Operation(int, Operation, int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> serializeRule(ArrayList&lt;Rule&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deserializedRule()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> deleteRule(Rule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> changeRule(Rule, Rule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> doesRuleExist(Rule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> toString()</t>
+  </si>
+  <si>
+    <t>SubRule</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getMetric()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getValue()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> passesSubRule(MethodMetrics)</t>
   </si>
   <si>
     <t>util</t>
   </si>
   <si>
+    <t>NumberTextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> replaceText(int, int, String)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> replaceSelection(String)</t>
+  </si>
+  <si>
     <t>Pair</t>
   </si>
   <si>
-    <t>public A getA()</t>
-  </si>
-  <si>
-    <t>public B getB()</t>
-  </si>
-  <si>
-    <t>public void setA(A a)</t>
-  </si>
-  <si>
-    <t>public void setB(B b)</t>
-  </si>
-  <si>
-    <t>NumberTextField</t>
-  </si>
-  <si>
-    <t>public void replaceText(int i, int i1, String string)</t>
-  </si>
-  <si>
-    <t>public void replaceSelection(String string)</t>
+    <t xml:space="preserve"> getA()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getB()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setA(A)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setB(B)</t>
   </si>
   <si>
     <t>Quadruple</t>
   </si>
   <si>
-    <t>public C getC()</t>
-  </si>
-  <si>
-    <t>public void setC(C c)</t>
-  </si>
-  <si>
-    <t>public D getD()</t>
-  </si>
-  <si>
-    <t>public void setD(D d)</t>
-  </si>
-  <si>
-    <t>rules</t>
-  </si>
-  <si>
-    <t>Rule</t>
-  </si>
-  <si>
-    <t>public SubRule getRule1()</t>
-  </si>
-  <si>
-    <t>public SubRule getRule2()</t>
-  </si>
-  <si>
-    <t>public LogicOp getOperation()</t>
-  </si>
-  <si>
-    <t>public Smell getSmell()</t>
-  </si>
-  <si>
-    <t>public Metric getMetric(SubRule sr)</t>
-  </si>
-  <si>
-    <t>public Operation getMetricOperation(SubRule sr)</t>
-  </si>
-  <si>
-    <t>public Integer getMetricValue(SubRule sr)</t>
-  </si>
-  <si>
-    <t>public boolean passesRule(MethodMetrics method) throws NoSuchElementException</t>
-  </si>
-  <si>
-    <t>private static boolean Operation(int value1, Operation op, int value2) throws NoSuchElementException</t>
-  </si>
-  <si>
-    <t>public static void serializeRule(ArrayList&lt;Rule&gt; rules) throws IOException</t>
-  </si>
-  <si>
-    <t>public static ArrayList&lt;Rule&gt; deserializedRule() throws IOException, ClassNotFoundException</t>
-  </si>
-  <si>
-    <t>public static void deleteRule(Rule r) throws IOException, ClassNotFoundException</t>
-  </si>
-  <si>
-    <t>public String toString()</t>
-  </si>
-  <si>
-    <t>SubRule</t>
-  </si>
-  <si>
-    <t>public Metric getMetric()</t>
-  </si>
-  <si>
-    <t>public Operation getOperation()</t>
-  </si>
-  <si>
-    <t>public Integer getValue()</t>
-  </si>
-  <si>
-    <t>private boolean passesSubRule(MethodMetrics method)</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>public ObservableList&lt;Rule&gt; getRegras()</t>
-  </si>
-  <si>
-    <t>private void initialize()</t>
-  </si>
-  <si>
-    <t>private void openProject()</t>
-  </si>
-  <si>
-    <t>private void createCodeSmell() throws IOException</t>
-  </si>
-  <si>
-    <t>private void addRuleToHistory() throws IOException, ClassNotFoundException</t>
-  </si>
-  <si>
-    <t>private void removeRuleFromHistory() throws IOException, ClassNotFoundException</t>
-  </si>
-  <si>
-    <t>private void clearGUIElements()</t>
-  </si>
-  <si>
-    <t>private void updateGUIElements(String pathCodeSmell)</t>
-  </si>
-  <si>
-    <t>private void writeCharacteristicsGUI(ArrayList&lt;String&gt; lines)</t>
-  </si>
-  <si>
-    <t>private void writeCodeSmellsGUI(ArrayList&lt;String&gt; lines)</t>
-  </si>
-  <si>
-    <t>public static void showInformationMessage(String title, String content, Alert.AlertType alertType)</t>
+    <t xml:space="preserve"> getC()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setC(C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getD()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setD(D)</t>
   </si>
   <si>
     <t>MetricExtractorTest</t>
   </si>
   <si>
-    <t xml:space="preserve"> static void setUpBeforeClass() throws IOException</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void setUp()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void testNom_Class() throws IOException</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void testCYCLO_method() throws IOException</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void testLOC_class() throws IOException</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> void testLOC_method() throws IOException</t>
+    <t xml:space="preserve"> setUpBeforeClass()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> setUp()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testNom_Class()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testCYCLO_method()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testLOC_class()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> testLOC_method()</t>
   </si>
   <si>
     <t>resources</t>
@@ -362,16 +419,16 @@
     <t>QuickSort</t>
   </si>
   <si>
-    <t>private int partition(int[] array, int low, int high)</t>
-  </si>
-  <si>
-    <t>private void quickSort(int[] array, int low, int high)</t>
+    <t xml:space="preserve"> partition(int[], int, int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> quickSort(int[], int, int)</t>
   </si>
   <si>
     <t>RuleTest</t>
   </si>
   <si>
-    <t xml:space="preserve"> void passesRuleTest() throws IllegalStateException</t>
+    <t xml:space="preserve"> passesRuleTest()</t>
   </si>
 </sst>
 </file>
@@ -416,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -471,13 +528,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F2" t="n">
-        <v>355.0</v>
+        <v>77.0</v>
       </c>
       <c r="G2" t="n">
-        <v>43.0</v>
+        <v>3.0</v>
       </c>
       <c r="H2" t="s">
         <v>14</v>
@@ -506,13 +563,13 @@
         <v>16</v>
       </c>
       <c r="E3" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F3" t="n">
-        <v>355.0</v>
+        <v>77.0</v>
       </c>
       <c r="G3" t="n">
-        <v>43.0</v>
+        <v>3.0</v>
       </c>
       <c r="H3" t="s">
         <v>14</v>
@@ -541,22 +598,22 @@
         <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F4" t="n">
-        <v>355.0</v>
+        <v>77.0</v>
       </c>
       <c r="G4" t="n">
-        <v>43.0</v>
+        <v>3.0</v>
       </c>
       <c r="H4" t="s">
         <v>14</v>
       </c>
       <c r="I4" t="n">
-        <v>15.0</v>
+        <v>26.0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -576,22 +633,22 @@
         <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F5" t="n">
-        <v>355.0</v>
+        <v>77.0</v>
       </c>
       <c r="G5" t="n">
-        <v>43.0</v>
+        <v>3.0</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="I5" t="n">
-        <v>19.0</v>
+        <v>6.0</v>
       </c>
       <c r="J5" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
@@ -605,25 +662,25 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F6" t="n">
-        <v>355.0</v>
+        <v>169.0</v>
       </c>
       <c r="G6" t="n">
-        <v>43.0</v>
+        <v>1.0</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
       </c>
       <c r="I6" t="n">
-        <v>11.0</v>
+        <v>4.0</v>
       </c>
       <c r="J6" t="n">
         <v>0.0</v>
@@ -640,28 +697,28 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F7" t="n">
-        <v>355.0</v>
+        <v>169.0</v>
       </c>
       <c r="G7" t="n">
-        <v>43.0</v>
+        <v>1.0</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I7" t="n">
-        <v>3.0</v>
+        <v>18.0</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K7" t="s">
         <v>15</v>
@@ -675,28 +732,28 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="F8" t="n">
-        <v>355.0</v>
+        <v>169.0</v>
       </c>
       <c r="G8" t="n">
-        <v>43.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="n">
-        <v>8.0</v>
+        <v>13.0</v>
       </c>
       <c r="J8" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
@@ -710,28 +767,28 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>169.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" t="n">
         <v>14.0</v>
       </c>
-      <c r="F9" t="n">
-        <v>355.0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" t="n">
-        <v>6.0</v>
-      </c>
       <c r="J9" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
@@ -742,31 +799,31 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E10" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F10" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G10" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
       </c>
       <c r="I10" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="J10" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K10" t="s">
         <v>15</v>
@@ -777,31 +834,31 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E11" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F11" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G11" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I11" t="n">
-        <v>39.0</v>
+        <v>31.0</v>
       </c>
       <c r="J11" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="K11" t="s">
         <v>15</v>
@@ -812,31 +869,31 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E12" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F12" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G12" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" t="n">
-        <v>41.0</v>
+        <v>17.0</v>
       </c>
       <c r="J12" t="n">
-        <v>13.0</v>
+        <v>2.0</v>
       </c>
       <c r="K12" t="s">
         <v>15</v>
@@ -847,31 +904,31 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E13" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F13" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G13" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
       </c>
       <c r="I13" t="n">
-        <v>17.0</v>
+        <v>5.0</v>
       </c>
       <c r="J13" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K13" t="s">
         <v>15</v>
@@ -882,31 +939,31 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E14" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F14" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G14" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H14" t="s">
         <v>14</v>
       </c>
       <c r="I14" t="n">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="J14" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="K14" t="s">
         <v>15</v>
@@ -917,22 +974,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E15" t="n">
-        <v>14.0</v>
+        <v>21.0</v>
       </c>
       <c r="F15" t="n">
-        <v>355.0</v>
+        <v>479.0</v>
       </c>
       <c r="G15" t="n">
-        <v>43.0</v>
+        <v>22.0</v>
       </c>
       <c r="H15" t="s">
         <v>14</v>
@@ -941,7 +998,7 @@
         <v>8.0</v>
       </c>
       <c r="J15" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K15" t="s">
         <v>15</v>
@@ -952,28 +1009,28 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E16" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F16" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G16" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H16" t="s">
         <v>14</v>
       </c>
       <c r="I16" t="n">
-        <v>3.0</v>
+        <v>8.0</v>
       </c>
       <c r="J16" t="n">
         <v>0.0</v>
@@ -987,22 +1044,22 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E17" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F17" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G17" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H17" t="s">
         <v>14</v>
@@ -1022,22 +1079,22 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E18" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F18" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G18" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -1057,31 +1114,31 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E19" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F19" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G19" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I19" t="n">
-        <v>3.0</v>
+        <v>28.0</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K19" t="s">
         <v>15</v>
@@ -1092,31 +1149,31 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E20" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F20" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G20" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
       </c>
       <c r="I20" t="n">
-        <v>21.0</v>
+        <v>16.0</v>
       </c>
       <c r="J20" t="n">
-        <v>6.0</v>
+        <v>3.0</v>
       </c>
       <c r="K20" t="s">
         <v>15</v>
@@ -1127,31 +1184,31 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E21" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F21" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G21" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
       </c>
       <c r="I21" t="n">
-        <v>16.0</v>
+        <v>10.0</v>
       </c>
       <c r="J21" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="K21" t="s">
         <v>15</v>
@@ -1162,31 +1219,31 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E22" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F22" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G22" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
       </c>
       <c r="I22" t="n">
-        <v>11.0</v>
+        <v>16.0</v>
       </c>
       <c r="J22" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K22" t="s">
         <v>15</v>
@@ -1197,31 +1254,31 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E23" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F23" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G23" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
       </c>
       <c r="I23" t="n">
-        <v>3.0</v>
+        <v>27.0</v>
       </c>
       <c r="J23" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K23" t="s">
         <v>15</v>
@@ -1232,31 +1289,31 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E24" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F24" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G24" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I24" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K24" t="s">
         <v>15</v>
@@ -1267,28 +1324,28 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E25" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F25" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G25" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H25" t="s">
         <v>14</v>
       </c>
       <c r="I25" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J25" t="n">
         <v>0.0</v>
@@ -1302,22 +1359,22 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E26" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F26" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G26" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H26" t="s">
         <v>14</v>
@@ -1337,28 +1394,28 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E27" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F27" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G27" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H27" t="s">
         <v>14</v>
       </c>
       <c r="I27" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="J27" t="n">
         <v>0.0</v>
@@ -1372,31 +1429,31 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E28" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F28" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G28" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H28" t="s">
         <v>14</v>
       </c>
       <c r="I28" t="n">
-        <v>3.0</v>
+        <v>24.0</v>
       </c>
       <c r="J28" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="K28" t="s">
         <v>15</v>
@@ -1407,31 +1464,31 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E29" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F29" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G29" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H29" t="s">
         <v>14</v>
       </c>
       <c r="I29" t="n">
-        <v>3.0</v>
+        <v>18.0</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K29" t="s">
         <v>15</v>
@@ -1442,28 +1499,28 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E30" t="n">
-        <v>17.0</v>
+        <v>21.0</v>
       </c>
       <c r="F30" t="n">
-        <v>148.0</v>
+        <v>479.0</v>
       </c>
       <c r="G30" t="n">
-        <v>15.0</v>
+        <v>22.0</v>
       </c>
       <c r="H30" t="s">
         <v>14</v>
       </c>
       <c r="I30" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J30" t="n">
         <v>0.0</v>
@@ -1477,28 +1534,28 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E31" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="F31" t="n">
-        <v>148.0</v>
+        <v>21.0</v>
       </c>
       <c r="G31" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I31" t="n">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="J31" t="n">
         <v>0.0</v>
@@ -1512,25 +1569,25 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E32" t="n">
-        <v>17.0</v>
+        <v>2.0</v>
       </c>
       <c r="F32" t="n">
-        <v>148.0</v>
+        <v>21.0</v>
       </c>
       <c r="G32" t="n">
-        <v>15.0</v>
+        <v>0.0</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I32" t="n">
         <v>3.0</v>
@@ -1547,28 +1604,28 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E33" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="F33" t="n">
-        <v>21.0</v>
+        <v>152.0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H33" t="s">
         <v>14</v>
       </c>
       <c r="I33" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="J33" t="n">
         <v>0.0</v>
@@ -1582,22 +1639,22 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E34" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="F34" t="n">
-        <v>21.0</v>
+        <v>152.0</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H34" t="s">
         <v>14</v>
@@ -1617,31 +1674,31 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
         <v>51</v>
       </c>
-      <c r="C35" t="s">
-        <v>52</v>
-      </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" t="n">
-        <v>1.0</v>
+        <v>17.0</v>
       </c>
       <c r="F35" t="n">
-        <v>23.0</v>
+        <v>152.0</v>
       </c>
       <c r="G35" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H35" t="s">
         <v>14</v>
       </c>
       <c r="I35" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="J35" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K35" t="s">
         <v>15</v>
@@ -1652,31 +1709,31 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
         <v>51</v>
-      </c>
-      <c r="C36" t="s">
-        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>55</v>
       </c>
       <c r="E36" t="n">
-        <v>1.0</v>
+        <v>17.0</v>
       </c>
       <c r="F36" t="n">
-        <v>45.0</v>
+        <v>152.0</v>
       </c>
       <c r="G36" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="H36" t="s">
         <v>14</v>
       </c>
       <c r="I36" t="n">
-        <v>27.0</v>
+        <v>3.0</v>
       </c>
       <c r="J36" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="K36" t="s">
         <v>15</v>
@@ -1687,31 +1744,31 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
         <v>56</v>
       </c>
-      <c r="D37" t="s">
-        <v>57</v>
-      </c>
       <c r="E37" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F37" t="n">
-        <v>161.0</v>
+        <v>152.0</v>
       </c>
       <c r="G37" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
       <c r="I37" t="n">
-        <v>4.0</v>
+        <v>21.0</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="K37" t="s">
         <v>15</v>
@@ -1722,31 +1779,31 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F38" t="n">
-        <v>161.0</v>
+        <v>152.0</v>
       </c>
       <c r="G38" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H38" t="s">
         <v>14</v>
       </c>
       <c r="I38" t="n">
-        <v>18.0</v>
+        <v>16.0</v>
       </c>
       <c r="J38" t="n">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="K38" t="s">
         <v>15</v>
@@ -1757,31 +1814,31 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F39" t="n">
-        <v>161.0</v>
+        <v>152.0</v>
       </c>
       <c r="G39" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H39" t="s">
         <v>14</v>
       </c>
       <c r="I39" t="n">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="J39" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K39" t="s">
         <v>15</v>
@@ -1792,28 +1849,28 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F40" t="n">
-        <v>161.0</v>
+        <v>152.0</v>
       </c>
       <c r="G40" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H40" t="s">
         <v>14</v>
       </c>
       <c r="I40" t="n">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="J40" t="n">
         <v>0.0</v>
@@ -1827,22 +1884,22 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E41" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F41" t="n">
-        <v>26.0</v>
+        <v>152.0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H41" t="s">
         <v>14</v>
@@ -1862,22 +1919,22 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" t="s">
         <v>61</v>
       </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" t="s">
-        <v>64</v>
-      </c>
       <c r="E42" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F42" t="n">
-        <v>26.0</v>
+        <v>152.0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H42" t="s">
         <v>14</v>
@@ -1897,22 +1954,22 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" t="s">
         <v>62</v>
       </c>
-      <c r="D43" t="s">
-        <v>65</v>
-      </c>
       <c r="E43" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F43" t="n">
-        <v>26.0</v>
+        <v>152.0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H43" t="s">
         <v>14</v>
@@ -1932,22 +1989,22 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E44" t="n">
-        <v>4.0</v>
+        <v>17.0</v>
       </c>
       <c r="F44" t="n">
-        <v>26.0</v>
+        <v>152.0</v>
       </c>
       <c r="G44" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H44" t="s">
         <v>14</v>
@@ -1967,31 +2024,31 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E45" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="F45" t="n">
-        <v>29.0</v>
+        <v>152.0</v>
       </c>
       <c r="G45" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H45" t="s">
         <v>14</v>
       </c>
       <c r="I45" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J45" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K45" t="s">
         <v>15</v>
@@ -2002,22 +2059,22 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E46" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="F46" t="n">
-        <v>29.0</v>
+        <v>152.0</v>
       </c>
       <c r="G46" t="n">
-        <v>1.0</v>
+        <v>15.0</v>
       </c>
       <c r="H46" t="s">
         <v>14</v>
@@ -2037,22 +2094,22 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E47" t="n">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="F47" t="n">
-        <v>74.0</v>
+        <v>152.0</v>
       </c>
       <c r="G47" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H47" t="s">
         <v>14</v>
@@ -2072,22 +2129,22 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E48" t="n">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="F48" t="n">
-        <v>74.0</v>
+        <v>152.0</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H48" t="s">
         <v>14</v>
@@ -2107,22 +2164,22 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C49" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E49" t="n">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="F49" t="n">
-        <v>74.0</v>
+        <v>152.0</v>
       </c>
       <c r="G49" t="n">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="H49" t="s">
         <v>14</v>
@@ -2142,22 +2199,22 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
         <v>70</v>
       </c>
-      <c r="D50" t="s">
-        <v>66</v>
-      </c>
       <c r="E50" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="F50" t="n">
-        <v>74.0</v>
+        <v>379.0</v>
       </c>
       <c r="G50" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="H50" t="s">
         <v>14</v>
@@ -2177,22 +2234,22 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
         <v>71</v>
       </c>
       <c r="E51" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="F51" t="n">
-        <v>74.0</v>
+        <v>379.0</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="H51" t="s">
         <v>14</v>
@@ -2212,28 +2269,28 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
         <v>72</v>
       </c>
       <c r="E52" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="F52" t="n">
-        <v>74.0</v>
+        <v>379.0</v>
       </c>
       <c r="G52" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="H52" t="s">
         <v>14</v>
       </c>
       <c r="I52" t="n">
-        <v>3.0</v>
+        <v>15.0</v>
       </c>
       <c r="J52" t="n">
         <v>0.0</v>
@@ -2247,31 +2304,31 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
         <v>73</v>
       </c>
       <c r="E53" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="F53" t="n">
-        <v>74.0</v>
+        <v>379.0</v>
       </c>
       <c r="G53" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="H53" t="s">
         <v>14</v>
       </c>
       <c r="I53" t="n">
-        <v>3.0</v>
+        <v>19.0</v>
       </c>
       <c r="J53" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="K53" t="s">
         <v>15</v>
@@ -2282,28 +2339,28 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
         <v>74</v>
       </c>
       <c r="E54" t="n">
-        <v>8.0</v>
+        <v>16.0</v>
       </c>
       <c r="F54" t="n">
-        <v>74.0</v>
+        <v>379.0</v>
       </c>
       <c r="G54" t="n">
-        <v>0.0</v>
+        <v>32.0</v>
       </c>
       <c r="H54" t="s">
         <v>14</v>
       </c>
       <c r="I54" t="n">
-        <v>3.0</v>
+        <v>11.0</v>
       </c>
       <c r="J54" t="n">
         <v>0.0</v>
@@ -2317,22 +2374,22 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D55" t="s">
         <v>75</v>
       </c>
-      <c r="C55" t="s">
-        <v>76</v>
-      </c>
-      <c r="D55" t="s">
-        <v>77</v>
-      </c>
       <c r="E55" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F55" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G55" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H55" t="s">
         <v>14</v>
@@ -2352,28 +2409,28 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" t="s">
         <v>76</v>
       </c>
-      <c r="D56" t="s">
-        <v>78</v>
-      </c>
       <c r="E56" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F56" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G56" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H56" t="s">
         <v>14</v>
       </c>
       <c r="I56" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J56" t="n">
         <v>0.0</v>
@@ -2387,31 +2444,31 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D57" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E57" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F57" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G57" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I57" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="J57" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K57" t="s">
         <v>15</v>
@@ -2422,28 +2479,28 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E58" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F58" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G58" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H58" t="s">
         <v>14</v>
       </c>
       <c r="I58" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="J58" t="n">
         <v>0.0</v>
@@ -2457,31 +2514,31 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C59" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E59" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F59" t="n">
+        <v>379.0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" t="n">
         <v>13.0</v>
       </c>
-      <c r="F59" t="n">
-        <v>232.0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="H59" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" t="n">
-        <v>3.0</v>
-      </c>
       <c r="J59" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K59" t="s">
         <v>15</v>
@@ -2492,31 +2549,31 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E60" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F60" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G60" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H60" t="s">
         <v>14</v>
       </c>
       <c r="I60" t="n">
-        <v>3.0</v>
+        <v>28.0</v>
       </c>
       <c r="J60" t="n">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="K60" t="s">
         <v>15</v>
@@ -2527,31 +2584,31 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E61" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F61" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G61" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H61" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I61" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="J61" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K61" t="s">
         <v>15</v>
@@ -2562,31 +2619,31 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C62" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E62" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F62" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G62" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H62" t="s">
         <v>14</v>
       </c>
       <c r="I62" t="n">
-        <v>14.0</v>
+        <v>30.0</v>
       </c>
       <c r="J62" t="n">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="K62" t="s">
         <v>15</v>
@@ -2597,31 +2654,31 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E63" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F63" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G63" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H63" t="s">
         <v>14</v>
       </c>
       <c r="I63" t="n">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="J63" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="K63" t="s">
         <v>15</v>
@@ -2632,31 +2689,31 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E64" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F64" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G64" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H64" t="s">
         <v>14</v>
       </c>
       <c r="I64" t="n">
-        <v>7.0</v>
+        <v>14.0</v>
       </c>
       <c r="J64" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="K64" t="s">
         <v>15</v>
@@ -2667,31 +2724,31 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D65" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E65" t="n">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="F65" t="n">
-        <v>232.0</v>
+        <v>379.0</v>
       </c>
       <c r="G65" t="n">
-        <v>13.0</v>
+        <v>32.0</v>
       </c>
       <c r="H65" t="s">
         <v>14</v>
       </c>
       <c r="I65" t="n">
-        <v>21.0</v>
+        <v>8.0</v>
       </c>
       <c r="J65" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K65" t="s">
         <v>15</v>
@@ -2702,31 +2759,31 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D66" t="s">
         <v>88</v>
       </c>
       <c r="E66" t="n">
-        <v>13.0</v>
+        <v>1.0</v>
       </c>
       <c r="F66" t="n">
-        <v>232.0</v>
+        <v>37.0</v>
       </c>
       <c r="G66" t="n">
-        <v>13.0</v>
+        <v>4.0</v>
       </c>
       <c r="H66" t="s">
         <v>14</v>
       </c>
       <c r="I66" t="n">
-        <v>8.0</v>
+        <v>26.0</v>
       </c>
       <c r="J66" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="K66" t="s">
         <v>15</v>
@@ -2737,31 +2794,31 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="D67" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F67" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>22</v>
+      </c>
+      <c r="I67" t="n">
         <v>13.0</v>
       </c>
-      <c r="F67" t="n">
-        <v>232.0</v>
-      </c>
-      <c r="G67" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="H67" t="s">
-        <v>14</v>
-      </c>
-      <c r="I67" t="n">
-        <v>3.0</v>
-      </c>
       <c r="J67" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K67" t="s">
         <v>15</v>
@@ -2772,22 +2829,22 @@
         <v>67.0</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D68" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E68" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="F68" t="n">
-        <v>25.0</v>
+        <v>370.0</v>
       </c>
       <c r="G68" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="H68" t="s">
         <v>14</v>
@@ -2807,22 +2864,22 @@
         <v>68.0</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E69" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="F69" t="n">
-        <v>25.0</v>
+        <v>370.0</v>
       </c>
       <c r="G69" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="H69" t="s">
         <v>14</v>
@@ -2842,22 +2899,22 @@
         <v>69.0</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E70" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="F70" t="n">
-        <v>25.0</v>
+        <v>370.0</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="H70" t="s">
         <v>14</v>
@@ -2877,28 +2934,28 @@
         <v>70.0</v>
       </c>
       <c r="B71" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C71" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D71" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E71" t="n">
-        <v>4.0</v>
+        <v>15.0</v>
       </c>
       <c r="F71" t="n">
-        <v>25.0</v>
+        <v>370.0</v>
       </c>
       <c r="G71" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="H71" t="s">
         <v>14</v>
       </c>
       <c r="I71" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="J71" t="n">
         <v>0.0</v>
@@ -2912,19 +2969,19 @@
         <v>71.0</v>
       </c>
       <c r="B72" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C72" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D72" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E72" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F72" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G72" t="n">
         <v>18.0</v>
@@ -2947,19 +3004,19 @@
         <v>72.0</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D73" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E73" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F73" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G73" t="n">
         <v>18.0</v>
@@ -2968,10 +3025,10 @@
         <v>14</v>
       </c>
       <c r="I73" t="n">
-        <v>32.0</v>
+        <v>3.0</v>
       </c>
       <c r="J73" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K73" t="s">
         <v>15</v>
@@ -2982,19 +3039,19 @@
         <v>73.0</v>
       </c>
       <c r="B74" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D74" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E74" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F74" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G74" t="n">
         <v>18.0</v>
@@ -3003,10 +3060,10 @@
         <v>14</v>
       </c>
       <c r="I74" t="n">
-        <v>14.0</v>
+        <v>3.0</v>
       </c>
       <c r="J74" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K74" t="s">
         <v>15</v>
@@ -3017,19 +3074,19 @@
         <v>74.0</v>
       </c>
       <c r="B75" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C75" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D75" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E75" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F75" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G75" t="n">
         <v>18.0</v>
@@ -3038,10 +3095,10 @@
         <v>14</v>
       </c>
       <c r="I75" t="n">
-        <v>27.0</v>
+        <v>14.0</v>
       </c>
       <c r="J75" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="K75" t="s">
         <v>15</v>
@@ -3052,19 +3109,19 @@
         <v>75.0</v>
       </c>
       <c r="B76" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C76" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D76" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E76" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F76" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G76" t="n">
         <v>18.0</v>
@@ -3073,10 +3130,10 @@
         <v>14</v>
       </c>
       <c r="I76" t="n">
-        <v>25.0</v>
+        <v>18.0</v>
       </c>
       <c r="J76" t="n">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="K76" t="s">
         <v>15</v>
@@ -3087,19 +3144,19 @@
         <v>76.0</v>
       </c>
       <c r="B77" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C77" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D77" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E77" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F77" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G77" t="n">
         <v>18.0</v>
@@ -3108,10 +3165,10 @@
         <v>14</v>
       </c>
       <c r="I77" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="J77" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K77" t="s">
         <v>15</v>
@@ -3122,19 +3179,19 @@
         <v>77.0</v>
       </c>
       <c r="B78" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C78" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D78" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E78" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F78" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G78" t="n">
         <v>18.0</v>
@@ -3143,7 +3200,7 @@
         <v>14</v>
       </c>
       <c r="I78" t="n">
-        <v>7.0</v>
+        <v>21.0</v>
       </c>
       <c r="J78" t="n">
         <v>0.0</v>
@@ -3157,19 +3214,19 @@
         <v>78.0</v>
       </c>
       <c r="B79" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D79" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E79" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F79" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G79" t="n">
         <v>18.0</v>
@@ -3178,10 +3235,10 @@
         <v>14</v>
       </c>
       <c r="I79" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="J79" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="K79" t="s">
         <v>15</v>
@@ -3192,19 +3249,19 @@
         <v>79.0</v>
       </c>
       <c r="B80" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D80" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E80" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F80" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G80" t="n">
         <v>18.0</v>
@@ -3213,10 +3270,10 @@
         <v>14</v>
       </c>
       <c r="I80" t="n">
-        <v>24.0</v>
+        <v>11.0</v>
       </c>
       <c r="J80" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="K80" t="s">
         <v>15</v>
@@ -3227,19 +3284,19 @@
         <v>80.0</v>
       </c>
       <c r="B81" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C81" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D81" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E81" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F81" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G81" t="n">
         <v>18.0</v>
@@ -3248,10 +3305,10 @@
         <v>14</v>
       </c>
       <c r="I81" t="n">
-        <v>18.0</v>
+        <v>10.0</v>
       </c>
       <c r="J81" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K81" t="s">
         <v>15</v>
@@ -3262,19 +3319,19 @@
         <v>81.0</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="C82" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D82" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E82" t="n">
-        <v>11.0</v>
+        <v>15.0</v>
       </c>
       <c r="F82" t="n">
-        <v>304.0</v>
+        <v>370.0</v>
       </c>
       <c r="G82" t="n">
         <v>18.0</v>
@@ -3283,7 +3340,7 @@
         <v>14</v>
       </c>
       <c r="I82" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="J82" t="n">
         <v>0.0</v>
@@ -3297,19 +3354,19 @@
         <v>82.0</v>
       </c>
       <c r="B83" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D83" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E83" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F83" t="n">
-        <v>76.0</v>
+        <v>53.0</v>
       </c>
       <c r="G83" t="n">
         <v>0.0</v>
@@ -3318,7 +3375,7 @@
         <v>14</v>
       </c>
       <c r="I83" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J83" t="n">
         <v>0.0</v>
@@ -3332,19 +3389,19 @@
         <v>83.0</v>
       </c>
       <c r="B84" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C84" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D84" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E84" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F84" t="n">
-        <v>76.0</v>
+        <v>53.0</v>
       </c>
       <c r="G84" t="n">
         <v>0.0</v>
@@ -3353,7 +3410,7 @@
         <v>14</v>
       </c>
       <c r="I84" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="J84" t="n">
         <v>0.0</v>
@@ -3367,19 +3424,19 @@
         <v>84.0</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C85" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D85" t="s">
         <v>110</v>
       </c>
       <c r="E85" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F85" t="n">
-        <v>76.0</v>
+        <v>53.0</v>
       </c>
       <c r="G85" t="n">
         <v>0.0</v>
@@ -3388,7 +3445,7 @@
         <v>14</v>
       </c>
       <c r="I85" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J85" t="n">
         <v>0.0</v>
@@ -3402,19 +3459,19 @@
         <v>85.0</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C86" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D86" t="s">
         <v>111</v>
       </c>
       <c r="E86" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="F86" t="n">
-        <v>76.0</v>
+        <v>53.0</v>
       </c>
       <c r="G86" t="n">
         <v>0.0</v>
@@ -3423,7 +3480,7 @@
         <v>14</v>
       </c>
       <c r="I86" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="J86" t="n">
         <v>0.0</v>
@@ -3437,31 +3494,31 @@
         <v>86.0</v>
       </c>
       <c r="B87" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D87" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E87" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="F87" t="n">
-        <v>76.0</v>
+        <v>29.0</v>
       </c>
       <c r="G87" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H87" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I87" t="n">
         <v>5.0</v>
       </c>
       <c r="J87" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K87" t="s">
         <v>15</v>
@@ -3472,28 +3529,28 @@
         <v>87.0</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C88" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D88" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E88" t="n">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c r="F88" t="n">
-        <v>76.0</v>
+        <v>29.0</v>
       </c>
       <c r="G88" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H88" t="s">
         <v>14</v>
       </c>
       <c r="I88" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="J88" t="n">
         <v>0.0</v>
@@ -3507,31 +3564,31 @@
         <v>88.0</v>
       </c>
       <c r="B89" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C89" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D89" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E89" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F89" t="n">
-        <v>70.0</v>
+        <v>26.0</v>
       </c>
       <c r="G89" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H89" t="s">
         <v>14</v>
       </c>
       <c r="I89" t="n">
-        <v>16.0</v>
+        <v>3.0</v>
       </c>
       <c r="J89" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K89" t="s">
         <v>15</v>
@@ -3542,31 +3599,31 @@
         <v>89.0</v>
       </c>
       <c r="B90" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C90" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D90" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E90" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F90" t="n">
-        <v>70.0</v>
+        <v>26.0</v>
       </c>
       <c r="G90" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H90" t="s">
         <v>14</v>
       </c>
       <c r="I90" t="n">
-        <v>7.0</v>
+        <v>3.0</v>
       </c>
       <c r="J90" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="K90" t="s">
         <v>15</v>
@@ -3577,28 +3634,28 @@
         <v>90.0</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C91" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D91" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="E91" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="F91" t="n">
-        <v>70.0</v>
+        <v>26.0</v>
       </c>
       <c r="G91" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="H91" t="s">
         <v>14</v>
       </c>
       <c r="I91" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="J91" t="n">
         <v>0.0</v>
@@ -3612,28 +3669,28 @@
         <v>91.0</v>
       </c>
       <c r="B92" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="C92" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D92" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="E92" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F92" t="n">
-        <v>64.0</v>
+        <v>26.0</v>
       </c>
       <c r="G92" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="H92" t="s">
         <v>14</v>
       </c>
       <c r="I92" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="J92" t="n">
         <v>0.0</v>
@@ -3647,33 +3704,698 @@
         <v>92.0</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="C93" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" t="s">
+        <v>107</v>
+      </c>
+      <c r="E93" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H93" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J93" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>112</v>
+      </c>
+      <c r="C94" t="s">
+        <v>121</v>
+      </c>
+      <c r="D94" t="s">
+        <v>117</v>
+      </c>
+      <c r="E94" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F94" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H94" t="s">
+        <v>14</v>
+      </c>
+      <c r="I94" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" t="s">
+        <v>119</v>
+      </c>
+      <c r="E95" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F95" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H95" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" t="s">
+        <v>121</v>
+      </c>
+      <c r="D96" t="s">
         <v>118</v>
       </c>
-      <c r="D93" t="s">
-        <v>119</v>
-      </c>
-      <c r="E93" t="n">
+      <c r="E96" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F96" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H96" t="s">
+        <v>14</v>
+      </c>
+      <c r="I96" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>112</v>
+      </c>
+      <c r="C97" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" t="s">
+        <v>120</v>
+      </c>
+      <c r="E97" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F97" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H97" t="s">
+        <v>14</v>
+      </c>
+      <c r="I97" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J97" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="B98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C98" t="s">
+        <v>121</v>
+      </c>
+      <c r="D98" t="s">
+        <v>122</v>
+      </c>
+      <c r="E98" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F98" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H98" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>112</v>
+      </c>
+      <c r="C99" t="s">
+        <v>121</v>
+      </c>
+      <c r="D99" t="s">
+        <v>123</v>
+      </c>
+      <c r="E99" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H99" t="s">
+        <v>14</v>
+      </c>
+      <c r="I99" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>112</v>
+      </c>
+      <c r="C100" t="s">
+        <v>121</v>
+      </c>
+      <c r="D100" t="s">
+        <v>124</v>
+      </c>
+      <c r="E100" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H100" t="s">
+        <v>14</v>
+      </c>
+      <c r="I100" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J100" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>112</v>
+      </c>
+      <c r="C101" t="s">
+        <v>121</v>
+      </c>
+      <c r="D101" t="s">
+        <v>125</v>
+      </c>
+      <c r="E101" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="F101" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H101" t="s">
+        <v>14</v>
+      </c>
+      <c r="I101" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J101" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>50</v>
+      </c>
+      <c r="C102" t="s">
+        <v>126</v>
+      </c>
+      <c r="D102" t="s">
+        <v>127</v>
+      </c>
+      <c r="E102" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F102" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H102" t="s">
+        <v>14</v>
+      </c>
+      <c r="I102" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" t="s">
+        <v>126</v>
+      </c>
+      <c r="D103" t="s">
+        <v>128</v>
+      </c>
+      <c r="E103" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F103" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H103" t="s">
+        <v>14</v>
+      </c>
+      <c r="I103" t="n">
         <v>2.0</v>
       </c>
-      <c r="F93" t="n">
+      <c r="J103" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K103" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" t="s">
+        <v>126</v>
+      </c>
+      <c r="D104" t="s">
+        <v>129</v>
+      </c>
+      <c r="E104" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F104" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H104" t="s">
+        <v>14</v>
+      </c>
+      <c r="I104" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J104" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C105" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" t="s">
+        <v>130</v>
+      </c>
+      <c r="E105" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F105" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H105" t="s">
+        <v>14</v>
+      </c>
+      <c r="I105" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="J105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K105" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="B106" t="s">
+        <v>50</v>
+      </c>
+      <c r="C106" t="s">
+        <v>126</v>
+      </c>
+      <c r="D106" t="s">
+        <v>131</v>
+      </c>
+      <c r="E106" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F106" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H106" t="s">
+        <v>14</v>
+      </c>
+      <c r="I106" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="J106" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>50</v>
+      </c>
+      <c r="C107" t="s">
+        <v>126</v>
+      </c>
+      <c r="D107" t="s">
+        <v>132</v>
+      </c>
+      <c r="E107" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H107" t="s">
+        <v>14</v>
+      </c>
+      <c r="I107" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="J107" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="B108" t="s">
+        <v>133</v>
+      </c>
+      <c r="C108" t="s">
+        <v>134</v>
+      </c>
+      <c r="D108" t="s">
+        <v>135</v>
+      </c>
+      <c r="E108" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F108" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="G108" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H108" t="s">
+        <v>14</v>
+      </c>
+      <c r="I108" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="J108" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K108" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>133</v>
+      </c>
+      <c r="C109" t="s">
+        <v>134</v>
+      </c>
+      <c r="D109" t="s">
+        <v>136</v>
+      </c>
+      <c r="E109" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F109" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="G109" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H109" t="s">
+        <v>22</v>
+      </c>
+      <c r="I109" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="J109" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="K109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>133</v>
+      </c>
+      <c r="C110" t="s">
+        <v>134</v>
+      </c>
+      <c r="D110" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="F110" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="G110" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="H110" t="s">
+        <v>14</v>
+      </c>
+      <c r="I110" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="J110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="B111" t="s">
+        <v>91</v>
+      </c>
+      <c r="C111" t="s">
+        <v>137</v>
+      </c>
+      <c r="D111" t="s">
+        <v>127</v>
+      </c>
+      <c r="E111" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F111" t="n">
         <v>64.0</v>
       </c>
-      <c r="G93" t="n">
+      <c r="G111" t="n">
         <v>5.0</v>
       </c>
-      <c r="H93" t="s">
-        <v>14</v>
-      </c>
-      <c r="I93" t="n">
+      <c r="H111" t="s">
+        <v>14</v>
+      </c>
+      <c r="I111" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="J111" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>91</v>
+      </c>
+      <c r="C112" t="s">
+        <v>137</v>
+      </c>
+      <c r="D112" t="s">
+        <v>138</v>
+      </c>
+      <c r="E112" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F112" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="G112" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="H112" t="s">
+        <v>14</v>
+      </c>
+      <c r="I112" t="n">
         <v>23.0</v>
       </c>
-      <c r="J93" t="n">
+      <c r="J112" t="n">
         <v>5.0</v>
       </c>
-      <c r="K93" t="s">
+      <c r="K112" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>